<commit_message>
created a script with before/after plots and heatmaps of responses for the 3 pilots
</commit_message>
<xml_diff>
--- a/pilots.xlsx
+++ b/pilots.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>pilotID</t>
   </si>
@@ -36,11 +36,6 @@
   </si>
   <si>
     <t>My comment</t>
-  </si>
-  <si>
-    <t>Just schema consistent. 
-6/6 old/new PAs
-adjascent locations.</t>
   </si>
   <si>
     <t>Screen dirt served as a landmark!
@@ -48,6 +43,24 @@
 Bottom border easier, because of the word and picture serving as landmarks. Other borders also probably easier.
 Felt like new PAs were in the same loc as old. Might have had actual interference!
 Otherwise, didn't feel like old knowledge helped.</t>
+  </si>
+  <si>
+    <t>Just schema consistent. 
+6/6 old/new PAs
+adjascent locations.
+Small board</t>
+  </si>
+  <si>
+    <t>new2</t>
+  </si>
+  <si>
+    <t>new3</t>
+  </si>
+  <si>
+    <t>Larger board. But same as 48652</t>
+  </si>
+  <si>
+    <t>Larger board. 8/6 adjascent!</t>
   </si>
 </sst>
 </file>
@@ -371,16 +384,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -404,12 +417,28 @@
         <v>48652</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>